<commit_message>
Modifications to add extra space
Significant changes have been made to this version of the program, however further testing is recommended.
</commit_message>
<xml_diff>
--- a/Test_Files/Dye_Factorial_Test.xlsx
+++ b/Test_Files/Dye_Factorial_Test.xlsx
@@ -1,19 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10512"/>
+  <workbookPr defaultThemeVersion="166925"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Siddarth/Downloads/HSC_Generation_Pipeline-master/Test_Files/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FAC0ED2D-0CD5-1248-9E9B-708265760998}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView activeTab="0"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Dye Factorial Test" sheetId="1" r:id="rId2"/>
+    <sheet name="Dye Factorial Test" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="125725" fullCalcOnLoad="true"/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="70">
   <si>
     <t>Pattern</t>
   </si>
@@ -220,20 +227,25 @@
   </si>
   <si>
     <t>Growth</t>
+  </si>
+  <si>
+    <t>Block</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <name val="Calibri"/>
     </font>
     <font>
       <b/>
+      <sz val="11"/>
       <color indexed="8"/>
+      <name val="Calibri"/>
     </font>
   </fonts>
   <fills count="2">
@@ -252,339 +264,736 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border/>
-    <border/>
-    <border/>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="true" applyAlignment="true">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyAlignment="true">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyAlignment="true">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
+  <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+  <a:themeElements>
+    <a:clrScheme name="Office">
+      <a:dk1>
+        <a:sysClr val="windowText" lastClr="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="44546A"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="E7E6E6"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="4472C4"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="ED7D31"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="A5A5A5"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="FFC000"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="5B9BD5"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="70AD47"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0563C1"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="954F72"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Office">
+      <a:majorFont>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="游ゴシック Light"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="等线 Light"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="游ゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="等线"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme name="Office">
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="110000"/>
+                <a:satMod val="105000"/>
+                <a:tint val="67000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="103000"/>
+                <a:tint val="73000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="109000"/>
+                <a:tint val="81000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:satMod val="103000"/>
+                <a:lumMod val="102000"/>
+                <a:tint val="94000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:satMod val="110000"/>
+                <a:lumMod val="100000"/>
+                <a:shade val="100000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="99000"/>
+                <a:satMod val="120000"/>
+                <a:shade val="78000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="63000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:tint val="95000"/>
+            <a:satMod val="170000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="93000"/>
+                <a:satMod val="150000"/>
+                <a:shade val="98000"/>
+                <a:lumMod val="102000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:tint val="98000"/>
+                <a:satMod val="130000"/>
+                <a:shade val="90000"/>
+                <a:lumMod val="103000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="63000"/>
+                <a:satMod val="120000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
+  <a:extLst>
+    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+    </a:ext>
+  </a:extLst>
+</a:theme>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E65"/>
-  <sheetFormatPr defaultRowHeight="15"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:F65"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E68" sqref="E68"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="3">
-        <v>2</v>
+      <c r="B2" s="5">
+        <v>1</v>
       </c>
       <c r="C2" s="3">
         <v>2</v>
       </c>
       <c r="D2" s="3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3">
+        <v>2</v>
+      </c>
+      <c r="E2" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="3">
-        <v>4</v>
+      <c r="B3" s="5">
+        <v>1</v>
       </c>
       <c r="C3" s="3">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D3" s="3">
         <v>2</v>
       </c>
-    </row>
-    <row r="4">
+      <c r="E3" s="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="3">
+      <c r="B4" s="5">
         <v>1</v>
       </c>
       <c r="C4" s="3">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D4" s="3">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="5">
+        <v>4</v>
+      </c>
+      <c r="E4" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="3">
-        <v>3</v>
+      <c r="B5" s="5">
+        <v>1</v>
       </c>
       <c r="C5" s="3">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D5" s="3">
         <v>1</v>
       </c>
-    </row>
-    <row r="6">
+      <c r="E5" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="3">
+      <c r="B6" s="5">
         <v>1</v>
       </c>
       <c r="C6" s="3">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D6" s="3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7">
+        <v>3</v>
+      </c>
+      <c r="E6" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B7" s="3">
-        <v>3</v>
+      <c r="B7" s="5">
+        <v>1</v>
       </c>
       <c r="C7" s="3">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D7" s="3">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="8">
+        <v>4</v>
+      </c>
+      <c r="E7" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B8" s="3">
+      <c r="B8" s="5">
         <v>1</v>
       </c>
       <c r="C8" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D8" s="3">
         <v>2</v>
       </c>
-    </row>
-    <row r="9">
+      <c r="E8" s="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B9" s="3">
-        <v>3</v>
+      <c r="B9" s="5">
+        <v>1</v>
       </c>
       <c r="C9" s="3">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D9" s="3">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="10">
+        <v>2</v>
+      </c>
+      <c r="E9" s="3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B10" s="3">
-        <v>3</v>
+      <c r="B10" s="5">
+        <v>1</v>
       </c>
       <c r="C10" s="3">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D10" s="3">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="11">
+        <v>1</v>
+      </c>
+      <c r="E10" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B11" s="3">
+      <c r="B11" s="5">
         <v>1</v>
       </c>
       <c r="C11" s="3">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D11" s="3">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="12">
+        <v>3</v>
+      </c>
+      <c r="E11" s="3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B12" s="3">
+      <c r="B12" s="5">
         <v>1</v>
       </c>
       <c r="C12" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D12" s="3">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="13">
+        <v>2</v>
+      </c>
+      <c r="E12" s="3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B13" s="3">
-        <v>3</v>
+      <c r="B13" s="5">
+        <v>1</v>
       </c>
       <c r="C13" s="3">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D13" s="3">
         <v>2</v>
       </c>
-    </row>
-    <row r="14">
+      <c r="E13" s="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B14" s="3">
-        <v>3</v>
+      <c r="B14" s="5">
+        <v>1</v>
       </c>
       <c r="C14" s="3">
         <v>3</v>
       </c>
       <c r="D14" s="3">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="15">
+        <v>3</v>
+      </c>
+      <c r="E14" s="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="B15" s="3">
-        <v>4</v>
+      <c r="B15" s="5">
+        <v>1</v>
       </c>
       <c r="C15" s="3">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D15" s="3">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="16">
+        <v>3</v>
+      </c>
+      <c r="E15" s="3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="B16" s="3">
-        <v>3</v>
+      <c r="B16" s="5">
+        <v>1</v>
       </c>
       <c r="C16" s="3">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D16" s="3">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="17">
+        <v>1</v>
+      </c>
+      <c r="E16" s="3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B17" s="3">
-        <v>2</v>
+      <c r="B17" s="5">
+        <v>1</v>
       </c>
       <c r="C17" s="3">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D17" s="3">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="18">
+        <v>4</v>
+      </c>
+      <c r="E17" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A18" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="B18" s="3">
+      <c r="B18" s="5">
         <v>1</v>
       </c>
       <c r="C18" s="3">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D18" s="3">
         <v>4</v>
       </c>
-    </row>
-    <row r="19">
+      <c r="E18" s="3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A19" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="B19" s="3">
-        <v>3</v>
+      <c r="B19" s="5">
+        <v>1</v>
       </c>
       <c r="C19" s="3">
         <v>3</v>
       </c>
       <c r="D19" s="3">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="20">
+        <v>3</v>
+      </c>
+      <c r="E19" s="3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A20" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="B20" s="3">
-        <v>4</v>
+      <c r="B20" s="5">
+        <v>1</v>
       </c>
       <c r="C20" s="3">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="D20" s="3">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="21">
+        <v>1</v>
+      </c>
+      <c r="E20" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A21" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="B21" s="3">
-        <v>4</v>
+      <c r="B21" s="5">
+        <v>1</v>
       </c>
       <c r="C21" s="3">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D21" s="3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="22">
+        <v>2</v>
+      </c>
+      <c r="E21" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A22" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="B22" s="3">
-        <v>4</v>
+      <c r="B22" s="5">
+        <v>1</v>
       </c>
       <c r="C22" s="3">
         <v>4</v>
@@ -592,55 +1001,67 @@
       <c r="D22" s="3">
         <v>4</v>
       </c>
-    </row>
-    <row r="23">
+      <c r="E22" s="3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A23" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="B23" s="3">
-        <v>2</v>
+      <c r="B23" s="5">
+        <v>1</v>
       </c>
       <c r="C23" s="3">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D23" s="3">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="24">
+        <v>3</v>
+      </c>
+      <c r="E23" s="3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A24" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="B24" s="3">
-        <v>4</v>
+      <c r="B24" s="5">
+        <v>1</v>
       </c>
       <c r="C24" s="3">
         <v>4</v>
       </c>
       <c r="D24" s="3">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="25">
+        <v>4</v>
+      </c>
+      <c r="E24" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A25" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="B25" s="3">
-        <v>4</v>
+      <c r="B25" s="5">
+        <v>1</v>
       </c>
       <c r="C25" s="3">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D25" s="3">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="26">
+        <v>2</v>
+      </c>
+      <c r="E25" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A26" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="B26" s="3">
-        <v>2</v>
+      <c r="B26" s="5">
+        <v>1</v>
       </c>
       <c r="C26" s="3">
         <v>2</v>
@@ -648,376 +1069,457 @@
       <c r="D26" s="3">
         <v>2</v>
       </c>
-    </row>
-    <row r="27">
+      <c r="E26" s="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A27" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="B27" s="3">
+      <c r="B27" s="5">
         <v>1</v>
       </c>
       <c r="C27" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D27" s="3">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="28">
+        <v>2</v>
+      </c>
+      <c r="E27" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A28" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="B28" s="3">
+      <c r="B28" s="5">
         <v>1</v>
       </c>
       <c r="C28" s="3">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D28" s="3">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="29">
+        <v>4</v>
+      </c>
+      <c r="E28" s="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A29" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="B29" s="3">
-        <v>3</v>
+      <c r="B29" s="5">
+        <v>1</v>
       </c>
       <c r="C29" s="3">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D29" s="3">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="30">
+        <v>2</v>
+      </c>
+      <c r="E29" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A30" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="B30" s="3">
-        <v>3</v>
+      <c r="B30" s="5">
+        <v>1</v>
       </c>
       <c r="C30" s="3">
         <v>3</v>
       </c>
       <c r="D30" s="3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="31">
+        <v>3</v>
+      </c>
+      <c r="E30" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A31" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="B31" s="3">
-        <v>2</v>
+      <c r="B31" s="5">
+        <v>1</v>
       </c>
       <c r="C31" s="3">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D31" s="3">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="32">
+        <v>3</v>
+      </c>
+      <c r="E31" s="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A32" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="B32" s="3">
-        <v>2</v>
+      <c r="B32" s="5">
+        <v>1</v>
       </c>
       <c r="C32" s="3">
         <v>2</v>
       </c>
       <c r="D32" s="3">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="33">
+        <v>2</v>
+      </c>
+      <c r="E32" s="3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A33" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="B33" s="3">
-        <v>2</v>
+      <c r="B33" s="5">
+        <v>1</v>
       </c>
       <c r="C33" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D33" s="3">
         <v>1</v>
       </c>
-    </row>
-    <row r="34">
+      <c r="E33" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A34" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="B34" s="3">
-        <v>4</v>
+      <c r="B34" s="5">
+        <v>1</v>
       </c>
       <c r="C34" s="3">
         <v>4</v>
       </c>
       <c r="D34" s="3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="35">
+        <v>4</v>
+      </c>
+      <c r="E34" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A35" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="B35" s="3">
-        <v>4</v>
+      <c r="B35" s="5">
+        <v>1</v>
       </c>
       <c r="C35" s="3">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D35" s="3">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="36">
+        <v>2</v>
+      </c>
+      <c r="E35" s="3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A36" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="B36" s="3">
-        <v>2</v>
+      <c r="B36" s="5">
+        <v>1</v>
       </c>
       <c r="C36" s="3">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D36" s="3">
         <v>4</v>
       </c>
-    </row>
-    <row r="37">
+      <c r="E36" s="3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A37" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="B37" s="3">
-        <v>3</v>
+      <c r="B37" s="5">
+        <v>1</v>
       </c>
       <c r="C37" s="3">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D37" s="3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="38">
+        <v>2</v>
+      </c>
+      <c r="E37" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A38" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="B38" s="3">
-        <v>2</v>
+      <c r="B38" s="5">
+        <v>1</v>
       </c>
       <c r="C38" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D38" s="3">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="39">
+        <v>1</v>
+      </c>
+      <c r="E38" s="3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A39" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="B39" s="3">
-        <v>2</v>
+      <c r="B39" s="5">
+        <v>1</v>
       </c>
       <c r="C39" s="3">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D39" s="3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="40">
+        <v>4</v>
+      </c>
+      <c r="E39" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A40" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="B40" s="3">
+      <c r="B40" s="5">
         <v>1</v>
       </c>
       <c r="C40" s="3">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D40" s="3">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="41">
+        <v>3</v>
+      </c>
+      <c r="E40" s="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A41" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="B41" s="3">
-        <v>2</v>
+      <c r="B41" s="5">
+        <v>1</v>
       </c>
       <c r="C41" s="3">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D41" s="3">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="42">
+        <v>4</v>
+      </c>
+      <c r="E41" s="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A42" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="B42" s="3">
-        <v>4</v>
+      <c r="B42" s="5">
+        <v>1</v>
       </c>
       <c r="C42" s="3">
         <v>4</v>
       </c>
       <c r="D42" s="3">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="43">
+        <v>4</v>
+      </c>
+      <c r="E42" s="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A43" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="B43" s="3">
-        <v>4</v>
+      <c r="B43" s="5">
+        <v>1</v>
       </c>
       <c r="C43" s="3">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="D43" s="3">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="44">
+        <v>1</v>
+      </c>
+      <c r="E43" s="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A44" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="B44" s="3">
-        <v>4</v>
+      <c r="B44" s="5">
+        <v>1</v>
       </c>
       <c r="C44" s="3">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="D44" s="3">
         <v>1</v>
       </c>
-    </row>
-    <row r="45">
+      <c r="E44" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A45" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="B45" s="3">
+      <c r="B45" s="5">
         <v>1</v>
       </c>
       <c r="C45" s="3">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D45" s="3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="46">
+        <v>4</v>
+      </c>
+      <c r="E45" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A46" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="B46" s="3">
+      <c r="B46" s="5">
         <v>1</v>
       </c>
       <c r="C46" s="3">
         <v>1</v>
       </c>
       <c r="D46" s="3">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="47">
+        <v>1</v>
+      </c>
+      <c r="E46" s="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A47" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="B47" s="3">
+      <c r="B47" s="5">
         <v>1</v>
       </c>
       <c r="C47" s="3">
         <v>1</v>
       </c>
       <c r="D47" s="3">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="48">
+        <v>1</v>
+      </c>
+      <c r="E47" s="3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A48" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="B48" s="3">
-        <v>2</v>
+      <c r="B48" s="5">
+        <v>1</v>
       </c>
       <c r="C48" s="3">
         <v>2</v>
       </c>
       <c r="D48" s="3">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="49">
+        <v>2</v>
+      </c>
+      <c r="E48" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A49" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="B49" s="3">
-        <v>4</v>
+      <c r="B49" s="5">
+        <v>1</v>
       </c>
       <c r="C49" s="3">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D49" s="3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="50">
+        <v>3</v>
+      </c>
+      <c r="E49" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A50" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="B50" s="3">
-        <v>2</v>
+      <c r="B50" s="5">
+        <v>1</v>
       </c>
       <c r="C50" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D50" s="3">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="51">
+        <v>1</v>
+      </c>
+      <c r="E50" s="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A51" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="B51" s="3">
-        <v>2</v>
+      <c r="B51" s="5">
+        <v>1</v>
       </c>
       <c r="C51" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D51" s="3">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="52">
+        <v>1</v>
+      </c>
+      <c r="E51" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A52" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="B52" s="3">
-        <v>4</v>
+      <c r="B52" s="5">
+        <v>1</v>
       </c>
       <c r="C52" s="3">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D52" s="3">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="53">
+        <v>3</v>
+      </c>
+      <c r="E52" s="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A53" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="B53" s="3">
+      <c r="B53" s="5">
         <v>1</v>
       </c>
       <c r="C53" s="3">
@@ -1026,111 +1528,135 @@
       <c r="D53" s="3">
         <v>1</v>
       </c>
-    </row>
-    <row r="54">
+      <c r="E53" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A54" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="B54" s="3">
+      <c r="B54" s="5">
         <v>2</v>
       </c>
       <c r="C54" s="3">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D54" s="3">
         <v>3</v>
       </c>
-    </row>
-    <row r="55">
+      <c r="E54" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A55" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="B55" s="3">
-        <v>3</v>
+      <c r="B55" s="5">
+        <v>2</v>
       </c>
       <c r="C55" s="3">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D55" s="3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="56">
+        <v>4</v>
+      </c>
+      <c r="E55" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A56" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="B56" s="3">
-        <v>3</v>
+      <c r="B56" s="5">
+        <v>2</v>
       </c>
       <c r="C56" s="3">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D56" s="3">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="57">
+        <v>1</v>
+      </c>
+      <c r="E56" s="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A57" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="B57" s="3">
-        <v>3</v>
+      <c r="B57" s="5">
+        <v>2</v>
       </c>
       <c r="C57" s="3">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D57" s="3">
         <v>4</v>
       </c>
-    </row>
-    <row r="58">
+      <c r="E57" s="3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A58" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="B58" s="3">
-        <v>1</v>
+      <c r="B58" s="5">
+        <v>2</v>
       </c>
       <c r="C58" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D58" s="3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="59">
+        <v>2</v>
+      </c>
+      <c r="E58" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A59" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="B59" s="3">
-        <v>1</v>
+      <c r="B59" s="5">
+        <v>2</v>
       </c>
       <c r="C59" s="3">
         <v>1</v>
       </c>
       <c r="D59" s="3">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="60">
+        <v>1</v>
+      </c>
+      <c r="E59" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A60" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="B60" s="3">
-        <v>4</v>
+      <c r="B60" s="5">
+        <v>2</v>
       </c>
       <c r="C60" s="3">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="D60" s="3">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="61">
+        <v>1</v>
+      </c>
+      <c r="E60" s="3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A61" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="B61" s="3">
-        <v>3</v>
+      <c r="B61" s="5">
+        <v>2</v>
       </c>
       <c r="C61" s="3">
         <v>3</v>
@@ -1138,63 +1664,79 @@
       <c r="D61" s="3">
         <v>3</v>
       </c>
-    </row>
-    <row r="62">
+      <c r="E61" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A62" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="B62" s="3">
-        <v>1</v>
+      <c r="B62" s="5">
+        <v>2</v>
       </c>
       <c r="C62" s="3">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D62" s="3">
         <v>3</v>
       </c>
-    </row>
-    <row r="63">
+      <c r="E62" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A63" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="B63" s="3">
+      <c r="B63" s="5">
         <v>2</v>
       </c>
       <c r="C63" s="3">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D63" s="3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="64">
+        <v>3</v>
+      </c>
+      <c r="E63" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A64" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="B64" s="3">
-        <v>4</v>
+      <c r="B64" s="5">
+        <v>2</v>
       </c>
       <c r="C64" s="3">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D64" s="3">
         <v>3</v>
       </c>
-    </row>
-    <row r="65">
+      <c r="E64" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A65" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="B65" s="3">
-        <v>3</v>
+      <c r="B65" s="5">
+        <v>2</v>
       </c>
       <c r="C65" s="3">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D65" s="3">
+        <v>4</v>
+      </c>
+      <c r="E65" s="3">
         <v>2</v>
       </c>
     </row>
   </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>